<commit_message>
Modify the result of v20
</commit_message>
<xml_diff>
--- a/Results/comparison_different_version.xlsx
+++ b/Results/comparison_different_version.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Next++\4E\Wanying\4EBaseMetal\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E946E213-9ED4-4D25-AF35-6CE15AA529C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3B2FEEF-E0D7-4AE5-8F41-321D30D4B6D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="-1630" yWindow="790" windowWidth="12590" windowHeight="9840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all_v14_res" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>lag</t>
   </si>
@@ -85,10 +85,6 @@
   </si>
   <si>
     <t>v18</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>v20</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -802,7 +798,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -899,6 +895,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1255,10 +1254,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y55"/>
+  <dimension ref="A1:AB55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="87" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="87" workbookViewId="0">
+      <selection activeCell="S1" sqref="S1:W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1268,7 +1267,7 @@
     <col min="11" max="11" width="8.6640625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:28" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C1" t="s">
         <v>0</v>
       </c>
@@ -1298,9 +1297,6 @@
       </c>
       <c r="L1" t="s">
         <v>14</v>
-      </c>
-      <c r="M1" t="s">
-        <v>15</v>
       </c>
       <c r="N1" s="40" t="s">
         <v>11</v>
@@ -1308,20 +1304,23 @@
       <c r="O1" s="40"/>
       <c r="P1" s="40"/>
       <c r="Q1" s="40"/>
-      <c r="R1" s="40" t="s">
+      <c r="R1" s="40"/>
+      <c r="S1" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="S1" s="40"/>
       <c r="T1" s="40"/>
       <c r="U1" s="40"/>
-      <c r="V1" s="40" t="s">
+      <c r="V1" s="40"/>
+      <c r="W1" s="40"/>
+      <c r="X1" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="W1" s="40"/>
-      <c r="X1" s="40"/>
       <c r="Y1" s="40"/>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z1" s="40"/>
+      <c r="AA1" s="40"/>
+      <c r="AB1" s="40"/>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2" s="40" t="s">
         <v>1</v>
       </c>
@@ -1360,7 +1359,7 @@
         <v>0.47899657704077248</v>
       </c>
       <c r="M2">
-        <v>0.52066853538468927</v>
+        <v>0.50247499304522358</v>
       </c>
       <c r="N2">
         <f>AVERAGE(I2,I11,I20,I29,I38,I47)</f>
@@ -1379,39 +1378,48 @@
         <v>0.5059796792874004</v>
       </c>
       <c r="R2">
+        <v>0.50177224990693325</v>
+      </c>
+      <c r="S2">
         <f>AVERAGE(I5,I14,I23,I32,I41,I50)</f>
         <v>0.49456225565890238</v>
       </c>
-      <c r="S2">
+      <c r="T2">
         <f>AVERAGE(J7,J16,J25,J34,J43,J52)</f>
         <v>0.49976741818562959</v>
       </c>
-      <c r="T2">
+      <c r="U2">
         <f>AVERAGE(K7,K16,K25,K34,K43,K52)</f>
         <v>0.50068581817057767</v>
       </c>
-      <c r="U2" s="19">
+      <c r="V2" s="41">
         <f>AVERAGE(L5,L14,L23,L32,L41,L50)</f>
         <v>0.50450065549601941</v>
       </c>
-      <c r="V2">
+      <c r="W2" s="19">
+        <v>0.51321537596778832</v>
+      </c>
+      <c r="X2">
         <f>AVERAGE(I10,I19,I28,I37,I46,I55)</f>
         <v>0.52005499480575634</v>
       </c>
-      <c r="W2">
+      <c r="Y2">
         <f>AVERAGE(J8,J17,J26,J35,J44,J53)</f>
         <v>0.52120648057433627</v>
       </c>
-      <c r="X2" s="19">
+      <c r="Z2" s="19">
         <f>AVERAGE(K8,K17,K26,K35,K44,K53)</f>
         <v>0.53653336175719912</v>
       </c>
-      <c r="Y2">
+      <c r="AA2">
         <f>AVERAGE(L8,L17,L26,L35,L44,L53)</f>
         <v>0.52630261775073761</v>
       </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="AB2">
+        <v>0.511885695067686</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A3" s="40"/>
       <c r="B3" s="40"/>
       <c r="C3">
@@ -1446,10 +1454,10 @@
         <v>0.49501700392289621</v>
       </c>
       <c r="M3" s="19">
-        <v>0.52868542641847127</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+        <v>0.48685572569557828</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="40"/>
       <c r="B4" s="40"/>
       <c r="C4">
@@ -1484,10 +1492,10 @@
         <v>0.49884087069761379</v>
       </c>
       <c r="M4">
-        <v>0.52851054908458972</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+        <v>0.4990641290806388</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A5" s="40"/>
       <c r="B5" s="40">
         <v>3</v>
@@ -1524,10 +1532,10 @@
         <v>0.47282547342872405</v>
       </c>
       <c r="M5">
-        <v>0.46674432832992596</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+        <v>0.51892177792292049</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A6" s="40"/>
       <c r="B6" s="40"/>
       <c r="C6">
@@ -1561,11 +1569,11 @@
       <c r="L6" s="25">
         <v>0.48287184868020477</v>
       </c>
-      <c r="M6" s="19">
-        <v>0.50863500933351025</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="M6">
+        <v>0.51497065890957128</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="40"/>
       <c r="B7" s="40"/>
       <c r="C7">
@@ -1599,11 +1607,11 @@
       <c r="L7" s="21">
         <v>0.50711302216255194</v>
       </c>
-      <c r="M7">
-        <v>0.50885751176264193</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="M7" s="19">
+        <v>0.52687617676822596</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A8" s="40"/>
       <c r="B8" s="40">
         <v>5</v>
@@ -1640,10 +1648,10 @@
         <v>0.50319314924344072</v>
       </c>
       <c r="M8" s="19">
-        <v>0.53081394059613474</v>
-      </c>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+        <v>0.51697343275638907</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A9" s="40"/>
       <c r="B9" s="40"/>
       <c r="C9">
@@ -1678,10 +1686,10 @@
         <v>0.51292328378307506</v>
       </c>
       <c r="M9">
-        <v>0.50674840040156222</v>
-      </c>
-    </row>
-    <row r="10" spans="1:25" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+        <v>0.47271308828331904</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="40"/>
       <c r="B10" s="40"/>
       <c r="C10" s="2">
@@ -1716,10 +1724,10 @@
         <v>0.52267130923150695</v>
       </c>
       <c r="M10">
-        <v>0.49668413424128405</v>
-      </c>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
+        <v>0.5350545899504493</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A11" s="40" t="s">
         <v>2</v>
       </c>
@@ -1758,10 +1766,10 @@
         <v>0.47312684704734426</v>
       </c>
       <c r="M11">
-        <v>0.53119494135813627</v>
-      </c>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
+        <v>0.49495299982663399</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A12" s="40"/>
       <c r="B12" s="40"/>
       <c r="C12">
@@ -1796,10 +1804,10 @@
         <v>0.49290184493067379</v>
       </c>
       <c r="M12" s="19">
-        <v>0.53485955384609152</v>
-      </c>
-    </row>
-    <row r="13" spans="1:25" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+        <v>0.48712509726606679</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="40"/>
       <c r="B13" s="40"/>
       <c r="C13">
@@ -1834,10 +1842,10 @@
         <v>0.50110999229934927</v>
       </c>
       <c r="M13">
-        <v>0.54100470304115156</v>
-      </c>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
+        <v>0.51865240635243126</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A14" s="40"/>
       <c r="B14" s="40">
         <v>3</v>
@@ -1874,10 +1882,10 @@
         <v>0.43094436784111623</v>
       </c>
       <c r="M14">
-        <v>0.56921488644564522</v>
-      </c>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
+        <v>0.45245654777023803</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A15" s="40"/>
       <c r="B15" s="40"/>
       <c r="C15">
@@ -1911,11 +1919,11 @@
       <c r="L15" s="21">
         <v>0.48514021432804699</v>
       </c>
-      <c r="M15" s="19">
-        <v>0.56315012034785927</v>
-      </c>
-    </row>
-    <row r="16" spans="1:25" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="M15">
+        <v>0.49133374457225076</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="40"/>
       <c r="B16" s="40"/>
       <c r="C16">
@@ -1949,8 +1957,8 @@
       <c r="L16" s="26">
         <v>0.47323545242328524</v>
       </c>
-      <c r="M16">
-        <v>0.52905307199503249</v>
+      <c r="M16" s="19">
+        <v>0.5127640294963125</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
@@ -1990,7 +1998,7 @@
         <v>0.49298298398184026</v>
       </c>
       <c r="M17" s="19">
-        <v>0.62510910934520258</v>
+        <v>0.48452108808979477</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
@@ -2028,7 +2036,7 @@
         <v>0.47722008539255151</v>
       </c>
       <c r="M18">
-        <v>0.59317106531038422</v>
+        <v>0.50085926759155053</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -2066,7 +2074,7 @@
         <v>0.51678142046760256</v>
       </c>
       <c r="M19">
-        <v>0.55073786139635728</v>
+        <v>0.532846448629405</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
@@ -2108,7 +2116,7 @@
         <v>0.49304547617031674</v>
       </c>
       <c r="M20">
-        <v>0.50725211767883827</v>
+        <v>0.50890438090399948</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
@@ -2146,7 +2154,7 @@
         <v>0.47120445629780094</v>
       </c>
       <c r="M21" s="19">
-        <v>0.50928613761989372</v>
+        <v>0.46731356161124976</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -2184,7 +2192,7 @@
         <v>0.52478193250037275</v>
       </c>
       <c r="M22">
-        <v>0.51530327862242975</v>
+        <v>0.49128460756921477</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
@@ -2224,7 +2232,7 @@
         <v>0.50479400760388748</v>
       </c>
       <c r="M23">
-        <v>0.51106262926811497</v>
+        <v>0.50316039124141698</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
@@ -2261,8 +2269,8 @@
       <c r="L24" s="21">
         <v>0.51301626611189644</v>
       </c>
-      <c r="M24" s="19">
-        <v>0.51309513730138523</v>
+      <c r="M24">
+        <v>0.48744360583959201</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -2299,8 +2307,8 @@
       <c r="L25" s="26">
         <v>0.48693610879285204</v>
       </c>
-      <c r="M25">
-        <v>0.47091719381851427</v>
+      <c r="M25" s="19">
+        <v>0.48882271772480002</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
@@ -2340,7 +2348,7 @@
         <v>0.51479804943736829</v>
       </c>
       <c r="M26" s="19">
-        <v>0.49284010869609002</v>
+        <v>0.47699758296341954</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
@@ -2378,7 +2386,7 @@
         <v>0.44910666408634348</v>
       </c>
       <c r="M27">
-        <v>0.46694742794247424</v>
+        <v>0.50698501397002782</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -2416,7 +2424,7 @@
         <v>0.50263878305534349</v>
       </c>
       <c r="M28">
-        <v>0.48903186496849149</v>
+        <v>0.43075613532179402</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
@@ -2458,7 +2466,7 @@
         <v>0.52300166108268675</v>
       </c>
       <c r="M29">
-        <v>0.52696991505094071</v>
+        <v>0.54690794699049672</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
@@ -2496,7 +2504,7 @@
         <v>0.53909869129262</v>
       </c>
       <c r="M30" s="19">
-        <v>0.54893969906987405</v>
+        <v>0.54317781849849367</v>
       </c>
     </row>
     <row r="31" spans="1:13" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -2534,7 +2542,7 @@
         <v>0.51511353419532191</v>
       </c>
       <c r="M31">
-        <v>0.53308230624397701</v>
+        <v>0.52711505819837001</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
@@ -2574,7 +2582,7 @@
         <v>0.54457482129249923</v>
       </c>
       <c r="M32">
-        <v>0.51852288625212117</v>
+        <v>0.51865240635243126</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.3">
@@ -2611,8 +2619,8 @@
       <c r="L33" s="21">
         <v>0.51449062818760527</v>
       </c>
-      <c r="M33" s="19">
-        <v>0.52898680003709142</v>
+      <c r="M33">
+        <v>0.51500190500380971</v>
       </c>
     </row>
     <row r="34" spans="1:13" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -2649,8 +2657,8 @@
       <c r="L34" s="26">
         <v>0.50487439070116202</v>
       </c>
-      <c r="M34">
-        <v>0.55470233559514726</v>
+      <c r="M34" s="19">
+        <v>0.5308288076893608</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.3">
@@ -2690,7 +2698,7 @@
         <v>0.5649445029048783</v>
       </c>
       <c r="M35" s="19">
-        <v>0.57108662828436729</v>
+        <v>0.56267311344146453</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.3">
@@ -2728,7 +2736,7 @@
         <v>0.53489155589422244</v>
       </c>
       <c r="M36">
-        <v>0.61480369389310174</v>
+        <v>0.54679934161455579</v>
       </c>
     </row>
     <row r="37" spans="1:13" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -2766,7 +2774,7 @@
         <v>0.52709867919735798</v>
       </c>
       <c r="M37">
-        <v>0.61718444468634903</v>
+        <v>0.51092202184404356</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.3">
@@ -2808,7 +2816,7 @@
         <v>0.50931965157581072</v>
       </c>
       <c r="M38">
-        <v>0.51919266140119502</v>
+        <v>0.53505081018098499</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.3">
@@ -2846,7 +2854,7 @@
         <v>0.49112762114413067</v>
       </c>
       <c r="M39" s="19">
-        <v>0.53316193338735818</v>
+        <v>0.5112085283694372</v>
       </c>
     </row>
     <row r="40" spans="1:13" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -2884,7 +2892,7 @@
         <v>0.49895249988912621</v>
       </c>
       <c r="M40">
-        <v>0.53284342481383318</v>
+        <v>0.49706362309550001</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.3">
@@ -2924,7 +2932,7 @@
         <v>0.55275247852082976</v>
       </c>
       <c r="M41">
-        <v>0.54101805822659221</v>
+        <v>0.54473331962536897</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.3">
@@ -2961,8 +2969,8 @@
       <c r="L42" s="21">
         <v>0.48720396845555525</v>
       </c>
-      <c r="M42" s="19">
-        <v>0.50900038704839268</v>
+      <c r="M42">
+        <v>0.52265341832270906</v>
       </c>
     </row>
     <row r="43" spans="1:13" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -2999,8 +3007,8 @@
       <c r="L43" s="26">
         <v>0.53493918098947257</v>
       </c>
-      <c r="M43">
-        <v>0.47718657143663451</v>
+      <c r="M43" s="19">
+        <v>0.52077865266841594</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.3">
@@ -3040,7 +3048,7 @@
         <v>0.57088050485624731</v>
       </c>
       <c r="M44" s="19">
-        <v>0.53894094891364319</v>
+        <v>0.49287362265200674</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.3">
@@ -3078,7 +3086,7 @@
         <v>0.54319646536118427</v>
       </c>
       <c r="M45">
-        <v>0.49884389451318523</v>
+        <v>0.54871946450242071</v>
       </c>
     </row>
     <row r="46" spans="1:13" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -3116,7 +3124,7 @@
         <v>0.55484974660425446</v>
       </c>
       <c r="M46">
-        <v>0.5247343074051225</v>
+        <v>0.50285901762279683</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.3">
@@ -3158,7 +3166,7 @@
         <v>0.52084416867246397</v>
       </c>
       <c r="M47">
-        <v>0.50704675020461099</v>
+        <v>0.50707875225274224</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.3">
@@ -3196,7 +3204,7 @@
         <v>0.49911175417588899</v>
       </c>
       <c r="M48" s="19">
-        <v>0.50061963020751399</v>
+        <v>0.51495276800077372</v>
       </c>
     </row>
     <row r="49" spans="1:13" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -3234,7 +3242,7 @@
         <v>0.49707924614261867</v>
       </c>
       <c r="M49">
-        <v>0.48109384512419778</v>
+        <v>0.5169368949849007</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.3">
@@ -3274,7 +3282,7 @@
         <v>0.52111278428906005</v>
       </c>
       <c r="M50">
-        <v>0.5492902096915302</v>
+        <v>0.51695251803201947</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.3">
@@ -3311,8 +3319,8 @@
       <c r="L51" s="21">
         <v>0.51909741121069475</v>
       </c>
-      <c r="M51" s="19">
-        <v>0.52884316879744819</v>
+      <c r="M51">
+        <v>0.52085752385790418</v>
       </c>
     </row>
     <row r="52" spans="1:13" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -3349,8 +3357,8 @@
       <c r="L52" s="26">
         <v>0.54254306921312234</v>
       </c>
-      <c r="M52">
-        <v>0.5054295128431523</v>
+      <c r="M52" s="19">
+        <v>0.49922187145961527</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.3">
@@ -3390,7 +3398,7 @@
         <v>0.51101651608065068</v>
       </c>
       <c r="M53" s="19">
-        <v>0.5213821558595495</v>
+        <v>0.53727533050304155</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.3">
@@ -3428,7 +3436,7 @@
         <v>0.52733529276582303</v>
       </c>
       <c r="M54">
-        <v>0.5370966733996958</v>
+        <v>0.55086133386552449</v>
       </c>
     </row>
     <row r="55" spans="1:13" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -3466,11 +3474,24 @@
         <v>0.54694146094641316</v>
       </c>
       <c r="M55">
-        <v>0.52690515500078572</v>
+        <v>0.56868874253621504</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="B47:B49"/>
+    <mergeCell ref="N1:R1"/>
+    <mergeCell ref="S1:W1"/>
+    <mergeCell ref="X1:AB1"/>
+    <mergeCell ref="A2:A10"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="A11:A19"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="B17:B19"/>
     <mergeCell ref="B53:B55"/>
     <mergeCell ref="A20:A28"/>
     <mergeCell ref="A29:A37"/>
@@ -3485,19 +3506,6 @@
     <mergeCell ref="B38:B40"/>
     <mergeCell ref="B41:B43"/>
     <mergeCell ref="B50:B52"/>
-    <mergeCell ref="A2:A10"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="A11:A19"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="R1:U1"/>
-    <mergeCell ref="V1:Y1"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="B47:B49"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>